<commit_message>
add central friant wb
</commit_message>
<xml_diff>
--- a/gui_key.xlsx
+++ b/gui_key.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="8856" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="8856" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="input_data" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="586">
   <si>
     <t>Object List</t>
   </si>
@@ -1776,6 +1776,24 @@
   </si>
   <si>
     <t>Recovery of Groundwater for Banking Partner</t>
+  </si>
+  <si>
+    <t>northfriantwb</t>
+  </si>
+  <si>
+    <t>NFWB</t>
+  </si>
+  <si>
+    <t>North Friant WB</t>
+  </si>
+  <si>
+    <t>centralfriantwb</t>
+  </si>
+  <si>
+    <t>CFWB</t>
+  </si>
+  <si>
+    <t>Central Friant WB</t>
   </si>
 </sst>
 </file>
@@ -3310,8 +3328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3455,13 +3473,30 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>581</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>582</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>583</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>584</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -4502,7 +4537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>

</xml_diff>